<commit_message>
minor changes for F30, thresholding GB20240415
</commit_message>
<xml_diff>
--- a/ExcelFiles/s4_good_trials_GraspObject_4S_Action.xlsx
+++ b/ExcelFiles/s4_good_trials_GraspObject_4S_Action.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B5C74-1226-4E32-873C-AD2370A45033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB33CC6C-B6BA-4D97-B51C-F8905D63CDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +434,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20240415</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>